<commit_message>
chore: add type metadata for example custom type
</commit_message>
<xml_diff>
--- a/GameData/$CustomTypes.xlsx
+++ b/GameData/$CustomTypes.xlsx
@@ -23,7 +23,8 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
-    <t xml:space="preserve">namespace=TestGame</t>
+    <t xml:space="preserve">namespace=TestGame
+type=custom-type</t>
   </si>
   <si>
     <t xml:space="preserve">struct Reward</t>
@@ -41,7 +42,8 @@
     <t xml:space="preserve">int</t>
   </si>
   <si>
-    <t xml:space="preserve">namespace=TestGame.BattleSystem</t>
+    <t xml:space="preserve">namespace=TestGame.BattleSystem
+type=custom-type</t>
   </si>
   <si>
     <t xml:space="preserve">enum EnemyType</t>
@@ -185,7 +187,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -216,7 +218,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0546875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -224,7 +226,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.95"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -281,7 +283,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.03515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -290,7 +292,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="3" width="11.05"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>

</xml_diff>